<commit_message>
Created DDL code Staging DB, refact mapping doc json to STG - stg_norm(rank_name) 0 => "-", stg_norm(time) => '00:00:00.00
</commit_message>
<xml_diff>
--- a/Documents/Mapping documet json to DB Staging.xlsx
+++ b/Documents/Mapping documet json to DB Staging.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6237A7-7B05-47A3-BF1F-595A763FE940}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7879CD-97AB-4060-8130-2649E1472FA3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="source JSON schema" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="118">
   <si>
     <t>Key</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>result_id</t>
+  </si>
+  <si>
+    <t>00:00:00.00</t>
   </si>
 </sst>
 </file>
@@ -508,10 +511,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="47" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="47" fontId="0" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
@@ -906,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
@@ -2051,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6063E65B-5976-4536-AB87-9183F2F923C1}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2536,8 +2539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35A1A5A-F647-4F5F-87F4-EC634CFF10BD}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,7 +2638,7 @@
       <c r="I3" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2665,7 +2668,7 @@
       <c r="I4" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2693,7 +2696,7 @@
       <c r="I5" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2723,7 +2726,7 @@
       <c r="I6" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2751,7 +2754,7 @@
       <c r="I7" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2772,8 +2775,8 @@
       <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="3">
-        <v>0</v>
+      <c r="G8" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>9</v>
@@ -2781,7 +2784,7 @@
       <c r="I8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2800,8 +2803,8 @@
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="6">
-        <v>0</v>
+      <c r="G9" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>9</v>
@@ -2809,7 +2812,7 @@
       <c r="I9" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix mapping document - move stage attribute from event-entity into competition-entity
</commit_message>
<xml_diff>
--- a/Documents/Mapping documet json to DB Staging.xlsx
+++ b/Documents/Mapping documet json to DB Staging.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7879CD-97AB-4060-8130-2649E1472FA3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240290CE-3676-4588-BBED-AFDA72CC6D48}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="source JSON schema" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="118">
   <si>
     <t>Key</t>
   </si>
@@ -544,17 +544,110 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>163684</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>284724</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2">
+        <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D1DDC58-0519-43D9-9FB0-8BA53362A610}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D76129A8-D494-4BE7-B44A-3B455E23A8F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8209524" cy="5800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>65981</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>46958</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8562C08-A679-4F8F-96A3-29D865210143}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5762625"/>
+          <a:ext cx="5552381" cy="5333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>93110</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Рисунок 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10A4F9DD-FFC4-4A51-A12E-D9265C5A550E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -576,63 +669,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="7772400" cy="9117184"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>72795</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7ABD3497-8618-42FD-B60C-BF0384686B95}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="10058400" cy="7121295"/>
+          <a:off x="47625" y="47625"/>
+          <a:ext cx="10058400" cy="7093985"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -909,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,10 +975,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB4EFA7-6D41-4DB3-999C-A85F50D07C2D}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,27 +1085,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>26</v>
@@ -1075,56 +1111,30 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="H5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1137,7 +1147,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1321,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>9</v>
@@ -1357,7 +1367,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,8 +1487,8 @@
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>40</v>
+      <c r="G4" s="3">
+        <v>-1</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>9</v>
@@ -1524,7 +1534,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE6A627-9502-4D1E-981B-9B6248D593BD}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,57 +1892,55 @@
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>58</v>
+      <c r="G7" s="3">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3">
-        <v>30</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>26</v>
@@ -1940,7 +1948,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>57</v>
@@ -1949,7 +1957,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
@@ -1962,7 +1970,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>26</v>
@@ -1970,33 +1978,37 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
@@ -2014,33 +2026,59 @@
         <v>9</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="D12" s="3">
+        <v>50</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3" t="s">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2054,7 +2092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6063E65B-5976-4536-AB87-9183F2F923C1}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -2232,7 +2270,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>9</v>
@@ -2539,7 +2577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35A1A5A-F647-4F5F-87F4-EC634CFF10BD}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>